<commit_message>
Added gunicorn in requirements
</commit_message>
<xml_diff>
--- a/res/report-full-test.xlsx
+++ b/res/report-full-test.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\ConcreteFlowchartServer\res\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD09733A-ADA1-49F5-939C-BB88852D1FD7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="453" windowWidth="16500" windowHeight="6307" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>BIM Object ID</t>
   </si>
@@ -44,29 +39,79 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>40e526d7-263a-4f74-b935-1359b190b926</t>
+  </si>
+  <si>
+    <t>2018-09-10 04:59:51.285837</t>
+  </si>
+  <si>
+    <t>2018-09-10 05:00:09.798837</t>
+  </si>
+  <si>
+    <t>Casting</t>
+  </si>
+  <si>
+    <t>Casting: OK</t>
+  </si>
+  <si>
+    <t>2018-09-10 05:06:23.535176</t>
+  </si>
+  <si>
+    <t>2018-09-10 05:06:59.399146</t>
+  </si>
+  <si>
+    <t>Casting: Bad</t>
+  </si>
+  <si>
+    <t>2018-09-10 05:14:52.426060</t>
+  </si>
+  <si>
+    <t>2018-09-10 05:15:53.965341</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>2018-09-10 05:32:00.874461</t>
+  </si>
+  <si>
+    <t>2018-09-10 05:32:25.816646</t>
+  </si>
+  <si>
+    <t>2018-09-10 05:33:02.706576</t>
+  </si>
+  <si>
+    <t>26.2</t>
+  </si>
+  <si>
+    <t>25.8</t>
+  </si>
+  <si>
+    <t>24.8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -81,43 +126,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -405,19 +433,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
-  <cols>
-    <col min="8" max="8" width="13.9375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +472,137 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2" t="n">
+        <v>26</v>
+      </c>
+      <c r="F2" t="n">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="n">
+        <v>28</v>
+      </c>
+      <c r="E3" t="n">
+        <v>25.8</v>
+      </c>
+      <c r="F3" t="n">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="n">
+        <v>27.4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>24.8</v>
+      </c>
+      <c r="F4" t="n">
+        <v>24.6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="n">
+        <v>26.4</v>
+      </c>
+      <c r="E5" t="n">
+        <v>23.8</v>
+      </c>
+      <c r="F5" t="n">
+        <v>26.2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added explicit port 5000
</commit_message>
<xml_diff>
--- a/res/report-full-test.xlsx
+++ b/res/report-full-test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>BIM Object ID</t>
   </si>
@@ -71,25 +71,28 @@
     <t>2018-09-10 05:15:53.965341</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>2018-09-10 05:32:00.874461</t>
-  </si>
-  <si>
-    <t>2018-09-10 05:32:25.816646</t>
-  </si>
-  <si>
-    <t>2018-09-10 05:33:02.706576</t>
-  </si>
-  <si>
-    <t>26.2</t>
-  </si>
-  <si>
-    <t>25.8</t>
-  </si>
-  <si>
-    <t>24.8</t>
+    <t>Esame 2</t>
+  </si>
+  <si>
+    <t>2018-09-10 06:33:36.694791</t>
+  </si>
+  <si>
+    <t>2018-09-10 06:33:57.893403</t>
+  </si>
+  <si>
+    <t>2018-09-10 06:34:28.174998</t>
+  </si>
+  <si>
+    <t>20.0</t>
+  </si>
+  <si>
+    <t>40.0</t>
+  </si>
+  <si>
+    <t>Maturation</t>
+  </si>
+  <si>
+    <t>Maturation: OK</t>
   </si>
 </sst>
 </file>
@@ -561,19 +564,19 @@
         <v>20</v>
       </c>
       <c r="D5" t="n">
-        <v>26.4</v>
+        <v>20</v>
       </c>
       <c r="E5" t="n">
-        <v>23.8</v>
+        <v>28</v>
       </c>
       <c r="F5" t="n">
-        <v>26.2</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -593,13 +596,13 @@
         <v>23</v>
       </c>
       <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="s">
-        <v>11</v>
-      </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>